<commit_message>
Add SQL schema for course management system
Introduced initial SQL scripts to create tables for courses, departments, enrollments, students, and teachers. Also updated Lec_0_1.xlsx, likely to reflect schema changes or related content.
</commit_message>
<xml_diff>
--- a/Beginner/Slides/Lec_0_1.xlsx
+++ b/Beginner/Slides/Lec_0_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xiaotingzhou/Documents/Lectures/SQL/Beginner/Slides/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07746AB3-2CB7-A34B-9A8E-A500FFE99AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61DCAD4-567D-3144-875D-FB1A43B59F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" xr2:uid="{B01DC677-87C8-C645-902B-49FC9EAA203F}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18360" activeTab="3" xr2:uid="{B01DC677-87C8-C645-902B-49FC9EAA203F}"/>
   </bookViews>
   <sheets>
     <sheet name="SQL" sheetId="6" r:id="rId1"/>
@@ -476,9 +476,6 @@
     <t>🧱 3. 创建数据表</t>
   </si>
   <si>
-    <t>Create Tables</t>
-  </si>
-  <si>
     <t>有两种方法：</t>
   </si>
   <si>
@@ -604,6 +601,901 @@
     </r>
   </si>
   <si>
+    <t>关系类型</t>
+  </si>
+  <si>
+    <t>描述</t>
+  </si>
+  <si>
+    <t>学生 - 系部</t>
+  </si>
+  <si>
+    <t>每位学生属于一个系部（多对一）</t>
+  </si>
+  <si>
+    <t>课程 - 教师</t>
+  </si>
+  <si>
+    <t>每门课程由一位教师教授（多对一）</t>
+  </si>
+  <si>
+    <t>课程 - 系部</t>
+  </si>
+  <si>
+    <t>每门课程属于一个系部（多对一）</t>
+  </si>
+  <si>
+    <t>学生 - 课程</t>
+  </si>
+  <si>
+    <t>多对多，通过 enrollments 选课关系表完成连接</t>
+  </si>
+  <si>
+    <t>学生 - 成绩</t>
+  </si>
+  <si>
+    <t>enrollments 表记录学生在每门课程中的得分情况</t>
+  </si>
+  <si>
+    <t>🧩 基本组成</t>
+  </si>
+  <si>
+    <t>概念</t>
+  </si>
+  <si>
+    <t>说明</t>
+  </si>
+  <si>
+    <t>表（Table）</t>
+  </si>
+  <si>
+    <t>类似于 Excel 的一张表，每一行是记录，每一列是字段</t>
+  </si>
+  <si>
+    <t>行（Row）</t>
+  </si>
+  <si>
+    <t>表中的一条数据记录</t>
+  </si>
+  <si>
+    <t>列（Column）</t>
+  </si>
+  <si>
+    <t>表中的字段名，每列定义一个数据类型</t>
+  </si>
+  <si>
+    <t>主键（Primary Key）</t>
+  </si>
+  <si>
+    <t>唯一标识一行数据的字段</t>
+  </si>
+  <si>
+    <t>外键（Foreign Key）</t>
+  </si>
+  <si>
+    <t>指向其他表主键，用于建立表之间的关系</t>
+  </si>
+  <si>
+    <t>🔗 表之间的关系类型</t>
+  </si>
+  <si>
+    <t>一对一（1:1）</t>
+  </si>
+  <si>
+    <t>一对多（1:N）</t>
+  </si>
+  <si>
+    <t>多对多（M:N）</t>
+  </si>
+  <si>
+    <t>🧠 特点</t>
+  </si>
+  <si>
+    <t>🛠️ 常见关系型数据库管理系统（RDBMS）</t>
+  </si>
+  <si>
+    <t>系统名称</t>
+  </si>
+  <si>
+    <t>特点</t>
+  </si>
+  <si>
+    <t>MySQL</t>
+  </si>
+  <si>
+    <t>开源、轻量、常用于 Web 应用</t>
+  </si>
+  <si>
+    <t>PostgreSQL</t>
+  </si>
+  <si>
+    <t>开源、功能强大、支持复杂查询与扩展</t>
+  </si>
+  <si>
+    <t>SQLite</t>
+  </si>
+  <si>
+    <t>零配置、嵌入式、小型项目理想选择</t>
+  </si>
+  <si>
+    <t>Microsoft SQL Server</t>
+  </si>
+  <si>
+    <t>微软出品，常用于企业场景</t>
+  </si>
+  <si>
+    <t>Oracle</t>
+  </si>
+  <si>
+    <t>商业数据库中的旗舰产品，强大的性能与安全性支持</t>
+  </si>
+  <si>
+    <t>🌟 示例表关系（以学生选课为例）</t>
+  </si>
+  <si>
+    <t>students (学生表)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ↳ student_id (PK)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ↳ name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ↳ department_id (FK) → departments.department_id</t>
+  </si>
+  <si>
+    <t>departments (系部表)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ↳ department_id (PK)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ↳ department_name</t>
+  </si>
+  <si>
+    <t>courses (课程表)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ↳ course_id (PK)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ↳ teacher_id (FK)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ↳ department_id (FK)</t>
+  </si>
+  <si>
+    <t>teachers (教师表)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ↳ teacher_id (PK)</t>
+  </si>
+  <si>
+    <t>enrollments (选课表)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ↳ enrollment_id (PK)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ↳ student_id (FK)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ↳ course_id (FK)</t>
+  </si>
+  <si>
+    <r>
+      <t>结构化查询语言（SQL）</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Kai Regular"/>
+      </rPr>
+      <t>：用来操作数据，如 SELECT, INSERT, UPDATE, DELETE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>数据完整性约束</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Kai Regular"/>
+      </rPr>
+      <t>：如主键、外键、唯一、非空等</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>事务支持</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Kai Regular"/>
+      </rPr>
+      <t>：支持原子性、一致性、隔离性、持久性（ACID）</t>
+    </r>
+  </si>
+  <si>
+    <t>关系型数据库（Relational Database，简称 RDB）是一种使用表格（tables）结构来存储和管理数据的数据库系统。它的核心概念包括：</t>
+  </si>
+  <si>
+    <t>题目 1：查询所有年龄大于 21 岁的学生</t>
+  </si>
+  <si>
+    <t>✅ 初级题（简单筛选）</t>
+  </si>
+  <si>
+    <t>题目 2：查询性别为 Female 的学生</t>
+  </si>
+  <si>
+    <t>题目 3：查询学分为 4 的课程</t>
+  </si>
+  <si>
+    <t>✅ 中级题（组合条件 &amp; 模糊匹配）</t>
+  </si>
+  <si>
+    <t>题目 4：查询来自 Computer Science 系部，且年龄不小于 21 岁的学生</t>
+  </si>
+  <si>
+    <t>题目 5：查询课程名称中包含 “Writing” 的课程</t>
+  </si>
+  <si>
+    <t>题目 6：查询老师名字以 “Dr.” 开头的教师</t>
+  </si>
+  <si>
+    <t>题目 7：查询选课成绩在 80 到 90 分之间的选课记录</t>
+  </si>
+  <si>
+    <t>✅ 进阶题（IN, NOT IN, IS NULL, 多条件）</t>
+  </si>
+  <si>
+    <t>题目 8：查询课程 ID 是 201 或 203 的选课记录</t>
+  </si>
+  <si>
+    <t>题目 9：查询未指定系部的学生（假设允许 department_id 为空）</t>
+  </si>
+  <si>
+    <t>题目 10：查询课程学分不是 2 或 3 的课程</t>
+  </si>
+  <si>
+    <t>题目 11：查询未选修 SQL Basics 的学生 ID</t>
+  </si>
+  <si>
+    <t>✅ 高阶题（子查询 + WHERE）</t>
+  </si>
+  <si>
+    <t>题目 12：查询平均成绩高于 85 的学生信息</t>
+  </si>
+  <si>
+    <t>题目 13：查找选修课程总数为 2 门以上的学生</t>
+  </si>
+  <si>
+    <t>ER 图 （Entity-Relationship Model，实体关系模型）</t>
+  </si>
+  <si>
+    <t>数据类型</t>
+  </si>
+  <si>
+    <t>示例</t>
+  </si>
+  <si>
+    <t>INTEGER / INT</t>
+  </si>
+  <si>
+    <t>整数</t>
+  </si>
+  <si>
+    <t>1, 100</t>
+  </si>
+  <si>
+    <t>REAL / FLOAT</t>
+  </si>
+  <si>
+    <t>浮点数 / 小数</t>
+  </si>
+  <si>
+    <t>3.14, 99.99</t>
+  </si>
+  <si>
+    <t>TEXT</t>
+  </si>
+  <si>
+    <t>文本字符串</t>
+  </si>
+  <si>
+    <t>'Alice', '数学系'</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>日期</t>
+  </si>
+  <si>
+    <t>'2023-06-19'</t>
+  </si>
+  <si>
+    <t>TIME</t>
+  </si>
+  <si>
+    <t>时间</t>
+  </si>
+  <si>
+    <t>'12:30:00'</t>
+  </si>
+  <si>
+    <t>DATETIME</t>
+  </si>
+  <si>
+    <t>日期 + 时间</t>
+  </si>
+  <si>
+    <t>'2023-06-19 12:30:00'</t>
+  </si>
+  <si>
+    <t>BOOLEAN（部分数据库支持）</t>
+  </si>
+  <si>
+    <t>布尔值</t>
+  </si>
+  <si>
+    <t>IFNULL(x, default)</t>
+  </si>
+  <si>
+    <t>IFNULL(NULL, 0) → 0</t>
+  </si>
+  <si>
+    <t>SQL 常见数据类型表（Data Types）</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SQL 常用函数表（Functions）</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ↳ age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ↳ gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ↳score</t>
+  </si>
+  <si>
+    <t>📂 类别</t>
+  </si>
+  <si>
+    <t>语法 / 函数</t>
+  </si>
+  <si>
+    <t>📖 说明</t>
+  </si>
+  <si>
+    <t>✅ 范围判断</t>
+  </si>
+  <si>
+    <t>BETWEEN x AND y</t>
+  </si>
+  <si>
+    <t>score BETWEEN 80 AND 90</t>
+  </si>
+  <si>
+    <t>判断值是否在 x 到 y 之间（包含边界）</t>
+  </si>
+  <si>
+    <t>NOT BETWEEN x AND y</t>
+  </si>
+  <si>
+    <t>age NOT BETWEEN 10 AND 18</t>
+  </si>
+  <si>
+    <t>判断值不在 x 到 y 范围内</t>
+  </si>
+  <si>
+    <t>✅ 集合判断</t>
+  </si>
+  <si>
+    <t>IN (v1, v2, v3)</t>
+  </si>
+  <si>
+    <t>department_id IN (1, 2, 3)</t>
+  </si>
+  <si>
+    <t>判断值是否出现在给定集合中</t>
+  </si>
+  <si>
+    <t>NOT IN (v1, v2, v3)</t>
+  </si>
+  <si>
+    <t>gender NOT IN ('Male', 'Other')</t>
+  </si>
+  <si>
+    <t>判断值不在集合中</t>
+  </si>
+  <si>
+    <t>✅ 空值判断</t>
+  </si>
+  <si>
+    <t>IS NULL</t>
+  </si>
+  <si>
+    <t>score IS NULL</t>
+  </si>
+  <si>
+    <t>判断字段值是否为 NULL</t>
+  </si>
+  <si>
+    <t>IS NOT NULL</t>
+  </si>
+  <si>
+    <t>name IS NOT NULL</t>
+  </si>
+  <si>
+    <t>判断字段值不为 NULL</t>
+  </si>
+  <si>
+    <t>✅ 布尔逻辑</t>
+  </si>
+  <si>
+    <t>NOT 条件</t>
+  </si>
+  <si>
+    <t>NOT age &gt; 20</t>
+  </si>
+  <si>
+    <t>逻辑取反，条件不成立时为真</t>
+  </si>
+  <si>
+    <t>✅ 条件分支</t>
+  </si>
+  <si>
+    <t>CASE WHEN ... THEN ... END</t>
+  </si>
+  <si>
+    <t>CASE WHEN score &gt;= 90 THEN 'A' ELSE 'B' END</t>
+  </si>
+  <si>
+    <t>条件判断分类输出</t>
+  </si>
+  <si>
+    <t>✅ 空值处理</t>
+  </si>
+  <si>
+    <t>如果为 NULL，则替换为默认值</t>
+  </si>
+  <si>
+    <t>NULLIF(x, y)</t>
+  </si>
+  <si>
+    <t>NULLIF(5, 5) → NULL</t>
+  </si>
+  <si>
+    <t>若 x=y，返回 NULL，否则返回 x</t>
+  </si>
+  <si>
+    <t>COALESCE(x1, x2, ..., xn)</t>
+  </si>
+  <si>
+    <t>COALESCE(NULL, NULL, 'A') → 'A'</t>
+  </si>
+  <si>
+    <t>返回第一个非 NULL 的值</t>
+  </si>
+  <si>
+    <t>SQLite 常用逻辑函数与运算符汇总表</t>
+  </si>
+  <si>
+    <t xml:space="preserve">📂 类别 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 🧠 函数名 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ✅ 用法示例 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 📖 说明</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🔢 数学函数 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ROUND(x) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ROUND(88.678) → 89 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 四舍五入</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ABS(x) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ABS(-10) → 10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 绝对值</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CEIL(x) / FLOOR(x) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CEIL(3.4) → 4 / FLOOR(3.4) → 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 向上 / 向下取整</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> POWER(x, y) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> POWER(2, 3) → 8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> x 的 y 次幂</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SQRT(x) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SQRT(9) → 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 平方根</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RANDOM() </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RANDOM() → 随机整数 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 生成随机值</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🔠 字符串函数 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LENGTH(s) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LENGTH('SQL') → 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 字符串长度</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> UPPER(s) / LOWER(s) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> UPPER('sql') → 'SQL' </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 转换为大写 / 小写</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SUBSTR(s, start, len) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SUBSTR('SQL语言', 1, 3) → 'SQL' </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 截取子串</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TRIM(s) / LTRIM() / RTRIM() </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TRIM(' abc ') → 'abc' </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 去除空格/前导/尾部字符</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> REPLACE(s, old, new) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> REPLACE('apple', 'a', 'A') → 'Apple' </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 替换子串</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> INSTR(s, substr) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> INSTR('hello', 'e') → 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 查找子串位置</t>
+  </si>
+  <si>
+    <t xml:space="preserve">📅 日期函数 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DATE('now') </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DATE('now') → '2025-07-03' </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 当前日期</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DATETIME('now') </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DATETIME('now') → '2025-07-03 12:00:00' </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 当前日期时间</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> STRFTIME('%Y', 'now') </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> → '2025' </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 提取年份</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> STRFTIME('%m', 'now') </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> → '07' </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 提取月份</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> STRFTIME('%d', 'now') </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> → '03' </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 提取日</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> JULIANDAY('now') </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> → 2460473.5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 转换为儒略日</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🎯 聚合函数 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> COUNT(*) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> COUNT(*) → 10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 统计行数</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SUM(score) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SUM(score) → 285 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 求和</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AVG(score) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AVG(score) → 71.25 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 平均值</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MAX(score) / MIN(score) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MAX(score) → 95 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 最大值 / 最小值</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GROUP_CONCAT(column) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GROUP_CONCAT(name) → 'Tom,Jim,Amy' </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 分组合并字符串</t>
+  </si>
+  <si>
+    <t xml:space="preserve">🧠 逻辑函数 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CASE WHEN ... THEN ... ELSE ... END </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CASE WHEN score &gt; 90 THEN 'A' ELSE 'B' END </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 条件判断输出</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> IFNULL(x, default) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> IFNULL(NULL, 0) → 0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 空值替代</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NULLIF(x, y) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NULLIF(5, 5) → NULL / NULLIF(5, 3) → 5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 若相等返回 NULL，否则返回 x</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> COALESCE(x1, x2, ..., xn) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> COALESCE(NULL, NULL, 'OK') → 'OK' </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 返回第一个非 NULL 的值</t>
+  </si>
+  <si>
+    <t>😊 Welcome!! 欢迎来到SQ课程！</t>
+  </si>
+  <si>
+    <t>TRUE, FALSE (1, 0)</t>
+  </si>
+  <si>
+    <t>1 (True)</t>
+  </si>
+  <si>
+    <t>0 (False)</t>
+  </si>
+  <si>
+    <t>AND (并且)</t>
+  </si>
+  <si>
+    <t>OR （或者）</t>
+  </si>
+  <si>
+    <t>只要有一个是False，结果就是False</t>
+  </si>
+  <si>
+    <t>只要有一个True，结果就是True</t>
+  </si>
+  <si>
+    <t>-  ClimbAI Lab 讲师</t>
+  </si>
+  <si>
+    <t>技术用语确认/SQL Key words</t>
+  </si>
+  <si>
+    <t>Part 1: SQL 简介与语法规则</t>
+  </si>
+  <si>
+    <t>选择哪些字段</t>
+  </si>
+  <si>
+    <t>- SELECT</t>
+  </si>
+  <si>
+    <t>从哪个表中获取数据</t>
+  </si>
+  <si>
+    <t>查询条件</t>
+  </si>
+  <si>
+    <t>对列分组</t>
+  </si>
+  <si>
+    <t>分组后的条件</t>
+  </si>
+  <si>
+    <t>- GROUP BY</t>
+  </si>
+  <si>
+    <t>- HAVING</t>
+  </si>
+  <si>
+    <t>限制返回件数</t>
+  </si>
+  <si>
+    <t>- ORDER BY</t>
+  </si>
+  <si>
+    <t>- FROM</t>
+  </si>
+  <si>
+    <t>- WHERE</t>
+  </si>
+  <si>
+    <t>- JOIN</t>
+  </si>
+  <si>
+    <t>- ON</t>
+  </si>
+  <si>
+    <t>和另外一张表关联</t>
+  </si>
+  <si>
+    <t>关联条件</t>
+  </si>
+  <si>
+    <t>- LIMIT</t>
+  </si>
+  <si>
+    <t>👩‍🏫 About me: May  （周 晓婷）</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">关联其他表的字段；A field that links to another table’s </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Kai Regular"/>
+      </rPr>
+      <t>primary key</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Kai Regular"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>✅ 什么是 SQL（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Kai Regular"/>
+      </rPr>
+      <t>Structured Query Language</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Kai Regular"/>
+      </rPr>
+      <t>）？</t>
+    </r>
+  </si>
+  <si>
+    <t>Create Tables，Insert Data</t>
+  </si>
+  <si>
     <r>
       <t>这里我们推荐第一种，把目录下面</t>
     </r>
@@ -613,7 +1505,7 @@
         <color rgb="FFC00000"/>
         <rFont val="Kai Regular"/>
       </rPr>
-      <t>Creat_Table</t>
+      <t>Create_Table和Insert_Data</t>
     </r>
     <r>
       <rPr>
@@ -638,898 +1530,6 @@
         <rFont val="Kai Regular"/>
       </rPr>
       <t>到SQL编辑器中。</t>
-    </r>
-  </si>
-  <si>
-    <t>关系类型</t>
-  </si>
-  <si>
-    <t>描述</t>
-  </si>
-  <si>
-    <t>学生 - 系部</t>
-  </si>
-  <si>
-    <t>每位学生属于一个系部（多对一）</t>
-  </si>
-  <si>
-    <t>课程 - 教师</t>
-  </si>
-  <si>
-    <t>每门课程由一位教师教授（多对一）</t>
-  </si>
-  <si>
-    <t>课程 - 系部</t>
-  </si>
-  <si>
-    <t>每门课程属于一个系部（多对一）</t>
-  </si>
-  <si>
-    <t>学生 - 课程</t>
-  </si>
-  <si>
-    <t>多对多，通过 enrollments 选课关系表完成连接</t>
-  </si>
-  <si>
-    <t>学生 - 成绩</t>
-  </si>
-  <si>
-    <t>enrollments 表记录学生在每门课程中的得分情况</t>
-  </si>
-  <si>
-    <t>🧩 基本组成</t>
-  </si>
-  <si>
-    <t>概念</t>
-  </si>
-  <si>
-    <t>说明</t>
-  </si>
-  <si>
-    <t>表（Table）</t>
-  </si>
-  <si>
-    <t>类似于 Excel 的一张表，每一行是记录，每一列是字段</t>
-  </si>
-  <si>
-    <t>行（Row）</t>
-  </si>
-  <si>
-    <t>表中的一条数据记录</t>
-  </si>
-  <si>
-    <t>列（Column）</t>
-  </si>
-  <si>
-    <t>表中的字段名，每列定义一个数据类型</t>
-  </si>
-  <si>
-    <t>主键（Primary Key）</t>
-  </si>
-  <si>
-    <t>唯一标识一行数据的字段</t>
-  </si>
-  <si>
-    <t>外键（Foreign Key）</t>
-  </si>
-  <si>
-    <t>指向其他表主键，用于建立表之间的关系</t>
-  </si>
-  <si>
-    <t>🔗 表之间的关系类型</t>
-  </si>
-  <si>
-    <t>一对一（1:1）</t>
-  </si>
-  <si>
-    <t>一对多（1:N）</t>
-  </si>
-  <si>
-    <t>多对多（M:N）</t>
-  </si>
-  <si>
-    <t>🧠 特点</t>
-  </si>
-  <si>
-    <t>🛠️ 常见关系型数据库管理系统（RDBMS）</t>
-  </si>
-  <si>
-    <t>系统名称</t>
-  </si>
-  <si>
-    <t>特点</t>
-  </si>
-  <si>
-    <t>MySQL</t>
-  </si>
-  <si>
-    <t>开源、轻量、常用于 Web 应用</t>
-  </si>
-  <si>
-    <t>PostgreSQL</t>
-  </si>
-  <si>
-    <t>开源、功能强大、支持复杂查询与扩展</t>
-  </si>
-  <si>
-    <t>SQLite</t>
-  </si>
-  <si>
-    <t>零配置、嵌入式、小型项目理想选择</t>
-  </si>
-  <si>
-    <t>Microsoft SQL Server</t>
-  </si>
-  <si>
-    <t>微软出品，常用于企业场景</t>
-  </si>
-  <si>
-    <t>Oracle</t>
-  </si>
-  <si>
-    <t>商业数据库中的旗舰产品，强大的性能与安全性支持</t>
-  </si>
-  <si>
-    <t>🌟 示例表关系（以学生选课为例）</t>
-  </si>
-  <si>
-    <t>students (学生表)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ↳ student_id (PK)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ↳ name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ↳ department_id (FK) → departments.department_id</t>
-  </si>
-  <si>
-    <t>departments (系部表)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ↳ department_id (PK)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ↳ department_name</t>
-  </si>
-  <si>
-    <t>courses (课程表)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ↳ course_id (PK)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ↳ teacher_id (FK)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ↳ department_id (FK)</t>
-  </si>
-  <si>
-    <t>teachers (教师表)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ↳ teacher_id (PK)</t>
-  </si>
-  <si>
-    <t>enrollments (选课表)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ↳ enrollment_id (PK)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ↳ student_id (FK)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ↳ course_id (FK)</t>
-  </si>
-  <si>
-    <r>
-      <t>结构化查询语言（SQL）</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Kai Regular"/>
-      </rPr>
-      <t>：用来操作数据，如 SELECT, INSERT, UPDATE, DELETE</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>数据完整性约束</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Kai Regular"/>
-      </rPr>
-      <t>：如主键、外键、唯一、非空等</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>事务支持</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Kai Regular"/>
-      </rPr>
-      <t>：支持原子性、一致性、隔离性、持久性（ACID）</t>
-    </r>
-  </si>
-  <si>
-    <t>关系型数据库（Relational Database，简称 RDB）是一种使用表格（tables）结构来存储和管理数据的数据库系统。它的核心概念包括：</t>
-  </si>
-  <si>
-    <t>题目 1：查询所有年龄大于 21 岁的学生</t>
-  </si>
-  <si>
-    <t>✅ 初级题（简单筛选）</t>
-  </si>
-  <si>
-    <t>题目 2：查询性别为 Female 的学生</t>
-  </si>
-  <si>
-    <t>题目 3：查询学分为 4 的课程</t>
-  </si>
-  <si>
-    <t>✅ 中级题（组合条件 &amp; 模糊匹配）</t>
-  </si>
-  <si>
-    <t>题目 4：查询来自 Computer Science 系部，且年龄不小于 21 岁的学生</t>
-  </si>
-  <si>
-    <t>题目 5：查询课程名称中包含 “Writing” 的课程</t>
-  </si>
-  <si>
-    <t>题目 6：查询老师名字以 “Dr.” 开头的教师</t>
-  </si>
-  <si>
-    <t>题目 7：查询选课成绩在 80 到 90 分之间的选课记录</t>
-  </si>
-  <si>
-    <t>✅ 进阶题（IN, NOT IN, IS NULL, 多条件）</t>
-  </si>
-  <si>
-    <t>题目 8：查询课程 ID 是 201 或 203 的选课记录</t>
-  </si>
-  <si>
-    <t>题目 9：查询未指定系部的学生（假设允许 department_id 为空）</t>
-  </si>
-  <si>
-    <t>题目 10：查询课程学分不是 2 或 3 的课程</t>
-  </si>
-  <si>
-    <t>题目 11：查询未选修 SQL Basics 的学生 ID</t>
-  </si>
-  <si>
-    <t>✅ 高阶题（子查询 + WHERE）</t>
-  </si>
-  <si>
-    <t>题目 12：查询平均成绩高于 85 的学生信息</t>
-  </si>
-  <si>
-    <t>题目 13：查找选修课程总数为 2 门以上的学生</t>
-  </si>
-  <si>
-    <t>ER 图 （Entity-Relationship Model，实体关系模型）</t>
-  </si>
-  <si>
-    <t>数据类型</t>
-  </si>
-  <si>
-    <t>示例</t>
-  </si>
-  <si>
-    <t>INTEGER / INT</t>
-  </si>
-  <si>
-    <t>整数</t>
-  </si>
-  <si>
-    <t>1, 100</t>
-  </si>
-  <si>
-    <t>REAL / FLOAT</t>
-  </si>
-  <si>
-    <t>浮点数 / 小数</t>
-  </si>
-  <si>
-    <t>3.14, 99.99</t>
-  </si>
-  <si>
-    <t>TEXT</t>
-  </si>
-  <si>
-    <t>文本字符串</t>
-  </si>
-  <si>
-    <t>'Alice', '数学系'</t>
-  </si>
-  <si>
-    <t>DATE</t>
-  </si>
-  <si>
-    <t>日期</t>
-  </si>
-  <si>
-    <t>'2023-06-19'</t>
-  </si>
-  <si>
-    <t>TIME</t>
-  </si>
-  <si>
-    <t>时间</t>
-  </si>
-  <si>
-    <t>'12:30:00'</t>
-  </si>
-  <si>
-    <t>DATETIME</t>
-  </si>
-  <si>
-    <t>日期 + 时间</t>
-  </si>
-  <si>
-    <t>'2023-06-19 12:30:00'</t>
-  </si>
-  <si>
-    <t>BOOLEAN（部分数据库支持）</t>
-  </si>
-  <si>
-    <t>布尔值</t>
-  </si>
-  <si>
-    <t>IFNULL(x, default)</t>
-  </si>
-  <si>
-    <t>IFNULL(NULL, 0) → 0</t>
-  </si>
-  <si>
-    <t>SQL 常见数据类型表（Data Types）</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SQL 常用函数表（Functions）</t>
-  </si>
-  <si>
-    <t>Python</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ↳ age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ↳ gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ↳score</t>
-  </si>
-  <si>
-    <t>📂 类别</t>
-  </si>
-  <si>
-    <t>语法 / 函数</t>
-  </si>
-  <si>
-    <t>📖 说明</t>
-  </si>
-  <si>
-    <t>✅ 范围判断</t>
-  </si>
-  <si>
-    <t>BETWEEN x AND y</t>
-  </si>
-  <si>
-    <t>score BETWEEN 80 AND 90</t>
-  </si>
-  <si>
-    <t>判断值是否在 x 到 y 之间（包含边界）</t>
-  </si>
-  <si>
-    <t>NOT BETWEEN x AND y</t>
-  </si>
-  <si>
-    <t>age NOT BETWEEN 10 AND 18</t>
-  </si>
-  <si>
-    <t>判断值不在 x 到 y 范围内</t>
-  </si>
-  <si>
-    <t>✅ 集合判断</t>
-  </si>
-  <si>
-    <t>IN (v1, v2, v3)</t>
-  </si>
-  <si>
-    <t>department_id IN (1, 2, 3)</t>
-  </si>
-  <si>
-    <t>判断值是否出现在给定集合中</t>
-  </si>
-  <si>
-    <t>NOT IN (v1, v2, v3)</t>
-  </si>
-  <si>
-    <t>gender NOT IN ('Male', 'Other')</t>
-  </si>
-  <si>
-    <t>判断值不在集合中</t>
-  </si>
-  <si>
-    <t>✅ 空值判断</t>
-  </si>
-  <si>
-    <t>IS NULL</t>
-  </si>
-  <si>
-    <t>score IS NULL</t>
-  </si>
-  <si>
-    <t>判断字段值是否为 NULL</t>
-  </si>
-  <si>
-    <t>IS NOT NULL</t>
-  </si>
-  <si>
-    <t>name IS NOT NULL</t>
-  </si>
-  <si>
-    <t>判断字段值不为 NULL</t>
-  </si>
-  <si>
-    <t>✅ 布尔逻辑</t>
-  </si>
-  <si>
-    <t>NOT 条件</t>
-  </si>
-  <si>
-    <t>NOT age &gt; 20</t>
-  </si>
-  <si>
-    <t>逻辑取反，条件不成立时为真</t>
-  </si>
-  <si>
-    <t>✅ 条件分支</t>
-  </si>
-  <si>
-    <t>CASE WHEN ... THEN ... END</t>
-  </si>
-  <si>
-    <t>CASE WHEN score &gt;= 90 THEN 'A' ELSE 'B' END</t>
-  </si>
-  <si>
-    <t>条件判断分类输出</t>
-  </si>
-  <si>
-    <t>✅ 空值处理</t>
-  </si>
-  <si>
-    <t>如果为 NULL，则替换为默认值</t>
-  </si>
-  <si>
-    <t>NULLIF(x, y)</t>
-  </si>
-  <si>
-    <t>NULLIF(5, 5) → NULL</t>
-  </si>
-  <si>
-    <t>若 x=y，返回 NULL，否则返回 x</t>
-  </si>
-  <si>
-    <t>COALESCE(x1, x2, ..., xn)</t>
-  </si>
-  <si>
-    <t>COALESCE(NULL, NULL, 'A') → 'A'</t>
-  </si>
-  <si>
-    <t>返回第一个非 NULL 的值</t>
-  </si>
-  <si>
-    <t>SQLite 常用逻辑函数与运算符汇总表</t>
-  </si>
-  <si>
-    <t xml:space="preserve">📂 类别 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 🧠 函数名 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ✅ 用法示例 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 📖 说明</t>
-  </si>
-  <si>
-    <t xml:space="preserve">🔢 数学函数 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ROUND(x) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ROUND(88.678) → 89 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 四舍五入</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ABS(x) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ABS(-10) → 10 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 绝对值</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CEIL(x) / FLOOR(x) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CEIL(3.4) → 4 / FLOOR(3.4) → 3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 向上 / 向下取整</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> POWER(x, y) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> POWER(2, 3) → 8 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> x 的 y 次幂</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SQRT(x) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SQRT(9) → 3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 平方根</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RANDOM() </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> RANDOM() → 随机整数 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 生成随机值</t>
-  </si>
-  <si>
-    <t xml:space="preserve">🔠 字符串函数 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LENGTH(s) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LENGTH('SQL') → 3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 字符串长度</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> UPPER(s) / LOWER(s) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> UPPER('sql') → 'SQL' </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 转换为大写 / 小写</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SUBSTR(s, start, len) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SUBSTR('SQL语言', 1, 3) → 'SQL' </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 截取子串</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> TRIM(s) / LTRIM() / RTRIM() </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> TRIM(' abc ') → 'abc' </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 去除空格/前导/尾部字符</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> REPLACE(s, old, new) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> REPLACE('apple', 'a', 'A') → 'Apple' </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 替换子串</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> INSTR(s, substr) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> INSTR('hello', 'e') → 2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 查找子串位置</t>
-  </si>
-  <si>
-    <t xml:space="preserve">📅 日期函数 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DATE('now') </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DATE('now') → '2025-07-03' </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 当前日期</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DATETIME('now') </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DATETIME('now') → '2025-07-03 12:00:00' </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 当前日期时间</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> STRFTIME('%Y', 'now') </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> → '2025' </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 提取年份</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> STRFTIME('%m', 'now') </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> → '07' </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 提取月份</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> STRFTIME('%d', 'now') </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> → '03' </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 提取日</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> JULIANDAY('now') </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> → 2460473.5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 转换为儒略日</t>
-  </si>
-  <si>
-    <t xml:space="preserve">🎯 聚合函数 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> COUNT(*) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> COUNT(*) → 10 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 统计行数</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SUM(score) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SUM(score) → 285 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 求和</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> AVG(score) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> AVG(score) → 71.25 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 平均值</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> MAX(score) / MIN(score) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> MAX(score) → 95 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 最大值 / 最小值</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> GROUP_CONCAT(column) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> GROUP_CONCAT(name) → 'Tom,Jim,Amy' </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 分组合并字符串</t>
-  </si>
-  <si>
-    <t xml:space="preserve">🧠 逻辑函数 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CASE WHEN ... THEN ... ELSE ... END </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CASE WHEN score &gt; 90 THEN 'A' ELSE 'B' END </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 条件判断输出</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> IFNULL(x, default) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> IFNULL(NULL, 0) → 0 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 空值替代</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> NULLIF(x, y) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> NULLIF(5, 5) → NULL / NULLIF(5, 3) → 5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 若相等返回 NULL，否则返回 x</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> COALESCE(x1, x2, ..., xn) </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> COALESCE(NULL, NULL, 'OK') → 'OK' </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 返回第一个非 NULL 的值</t>
-  </si>
-  <si>
-    <t>😊 Welcome!! 欢迎来到SQ课程！</t>
-  </si>
-  <si>
-    <t>TRUE, FALSE (1, 0)</t>
-  </si>
-  <si>
-    <t>1 (True)</t>
-  </si>
-  <si>
-    <t>0 (False)</t>
-  </si>
-  <si>
-    <t>AND (并且)</t>
-  </si>
-  <si>
-    <t>OR （或者）</t>
-  </si>
-  <si>
-    <t>只要有一个是False，结果就是False</t>
-  </si>
-  <si>
-    <t>只要有一个True，结果就是True</t>
-  </si>
-  <si>
-    <t>-  ClimbAI Lab 讲师</t>
-  </si>
-  <si>
-    <t>技术用语确认/SQL Key words</t>
-  </si>
-  <si>
-    <t>Part 1: SQL 简介与语法规则</t>
-  </si>
-  <si>
-    <t>选择哪些字段</t>
-  </si>
-  <si>
-    <t>- SELECT</t>
-  </si>
-  <si>
-    <t>从哪个表中获取数据</t>
-  </si>
-  <si>
-    <t>查询条件</t>
-  </si>
-  <si>
-    <t>对列分组</t>
-  </si>
-  <si>
-    <t>分组后的条件</t>
-  </si>
-  <si>
-    <t>- GROUP BY</t>
-  </si>
-  <si>
-    <t>- HAVING</t>
-  </si>
-  <si>
-    <t>限制返回件数</t>
-  </si>
-  <si>
-    <t>- ORDER BY</t>
-  </si>
-  <si>
-    <t>- FROM</t>
-  </si>
-  <si>
-    <t>- WHERE</t>
-  </si>
-  <si>
-    <t>- JOIN</t>
-  </si>
-  <si>
-    <t>- ON</t>
-  </si>
-  <si>
-    <t>和另外一张表关联</t>
-  </si>
-  <si>
-    <t>关联条件</t>
-  </si>
-  <si>
-    <t>- LIMIT</t>
-  </si>
-  <si>
-    <t>👩‍🏫 About me: May  （周 晓婷）</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">关联其他表的字段；A field that links to another table’s </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Kai Regular"/>
-      </rPr>
-      <t>primary key</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Kai Regular"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>✅ 什么是 SQL（</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Kai Regular"/>
-      </rPr>
-      <t>Structured Query Language</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Kai Regular"/>
-      </rPr>
-      <t>）？</t>
     </r>
   </si>
 </sst>
@@ -4332,7 +4332,7 @@
   </sheetPr>
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -4343,7 +4343,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="32">
       <c r="A1" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="27">
@@ -4351,7 +4351,7 @@
     </row>
     <row r="3" spans="1:3" ht="27">
       <c r="A3" s="5" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="27">
@@ -4371,7 +4371,7 @@
     </row>
     <row r="7" spans="1:3" ht="27">
       <c r="A7" s="47" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="27">
@@ -4402,7 +4402,7 @@
     </row>
     <row r="17" spans="1:7" ht="27">
       <c r="A17" s="3" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30">
@@ -4491,7 +4491,7 @@
         <v>61</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="G25" s="15"/>
     </row>
@@ -4734,7 +4734,7 @@
     </row>
     <row r="53" spans="1:3" ht="27">
       <c r="A53" s="3" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>122</v>
@@ -4742,7 +4742,7 @@
     </row>
     <row r="55" spans="1:3" ht="23">
       <c r="A55" s="18" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="23">
@@ -4765,63 +4765,63 @@
     </row>
     <row r="60" spans="1:3" ht="23">
       <c r="A60" s="49" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B60" s="48" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="23">
       <c r="A61" s="49" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B61" s="48" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="23">
       <c r="A62" s="49" t="s">
+        <v>439</v>
+      </c>
+      <c r="B62" s="48" t="s">
         <v>441</v>
-      </c>
-      <c r="B62" s="48" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="23">
       <c r="A63" s="49" t="s">
+        <v>440</v>
+      </c>
+      <c r="B63" s="48" t="s">
         <v>442</v>
-      </c>
-      <c r="B63" s="48" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="23">
       <c r="A64" s="49" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B64" s="48" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="23">
       <c r="A65" s="49" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B65" s="48" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="23">
       <c r="A66" s="49" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B66" s="48" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="23">
       <c r="A67" s="49" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B67" s="48" t="s">
         <v>77</v>
@@ -4829,10 +4829,10 @@
     </row>
     <row r="68" spans="1:2" ht="23">
       <c r="A68" s="49" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B68" s="48" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="20">
@@ -4863,12 +4863,12 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19">
       <c r="A1" s="23" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="B4" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="17">
@@ -4879,7 +4879,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="B9" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="17">
@@ -4890,7 +4890,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="B14" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="17">
@@ -4898,12 +4898,12 @@
     </row>
     <row r="17" spans="1:2" ht="19">
       <c r="A17" s="23" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="B20" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="17">
@@ -4914,7 +4914,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="B25" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="17">
@@ -4925,7 +4925,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="B30" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="17">
@@ -4936,7 +4936,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="B35" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="17">
@@ -4947,12 +4947,12 @@
     </row>
     <row r="42" spans="1:2" ht="19">
       <c r="A42" s="23" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="B45" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="17">
@@ -4963,7 +4963,7 @@
     </row>
     <row r="50" spans="1:2">
       <c r="B50" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="17">
@@ -4974,7 +4974,7 @@
     </row>
     <row r="55" spans="1:2">
       <c r="B55" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="17">
@@ -4985,7 +4985,7 @@
     </row>
     <row r="60" spans="1:2">
       <c r="B60" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="17">
@@ -5005,12 +5005,12 @@
     </row>
     <row r="70" spans="1:2" ht="19">
       <c r="A70" s="23" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="B73" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="17">
@@ -5033,7 +5033,7 @@
     </row>
     <row r="82" spans="1:2">
       <c r="B82" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="17">
@@ -5088,252 +5088,252 @@
   <sheetData>
     <row r="1" spans="1:2" ht="25">
       <c r="A1" s="26" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="17" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="B4" s="17" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="B5" s="18" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="B6" s="18" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="B7" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="B8" s="18" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="B9" s="18" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="17" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="B12" s="17" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="B13" s="18" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="B14" s="18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="B15" s="18" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="17" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="B18" s="17" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="B20" s="17" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="B22" s="17" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="17" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="B26" s="27" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D26" s="27" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="B27" s="28" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="B28" s="28" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="B29" s="28" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="B30" s="28" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="B31" s="28" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="17" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="B38" s="35" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D38" s="30" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="B39" s="18" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C39" s="29" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="B40" s="18" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C40" s="60" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D40" s="61" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="C41" s="60" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D41" s="61" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="B42" s="37" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C42" s="29" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D42" s="50" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="B43" s="18" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D43" s="50" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="B44" s="38" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="B45" s="18" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="C46" s="67" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D46" s="67"/>
     </row>
     <row r="47" spans="1:4">
       <c r="B47" s="37" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="B48" s="38" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="49" spans="2:3">
@@ -5341,57 +5341,57 @@
     </row>
     <row r="50" spans="2:3">
       <c r="B50" s="39" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="51" spans="2:3">
       <c r="B51" s="18" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="52" spans="2:3">
       <c r="B52" s="18" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="53" spans="2:3">
       <c r="B53" s="18" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="54" spans="2:3">
       <c r="B54" s="18" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="56" spans="2:3">
       <c r="B56" s="35" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="57" spans="2:3">
       <c r="B57" s="18" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="58" spans="2:3">
       <c r="B58" s="18" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="59" spans="2:3">
       <c r="B59" s="18" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="60" spans="2:3">
       <c r="B60" s="18" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="61" spans="2:3">
       <c r="B61" s="36" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -5429,116 +5429,116 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="25" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="B3" s="27" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="B4" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>259</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>260</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="B5" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>262</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="B6" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>265</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="B7" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>268</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="B8" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>271</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>274</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="B10" s="7" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="J11" s="18" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="I12" s="18" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="25" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="I13" s="45" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="J13" s="45" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -5548,10 +5548,10 @@
       <c r="D14" s="42"/>
       <c r="E14" s="42"/>
       <c r="G14" s="18" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="H14" s="18" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="I14" s="18" t="b">
         <v>1</v>
@@ -5562,36 +5562,36 @@
     </row>
     <row r="15" spans="1:10">
       <c r="B15" s="43" t="s">
+        <v>285</v>
+      </c>
+      <c r="C15" s="43" t="s">
+        <v>286</v>
+      </c>
+      <c r="D15" s="43" t="s">
+        <v>256</v>
+      </c>
+      <c r="E15" s="43" t="s">
         <v>287</v>
-      </c>
-      <c r="C15" s="43" t="s">
-        <v>288</v>
-      </c>
-      <c r="D15" s="43" t="s">
-        <v>258</v>
-      </c>
-      <c r="E15" s="43" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="B16" s="71" t="s">
+        <v>288</v>
+      </c>
+      <c r="C16" s="40" t="s">
+        <v>289</v>
+      </c>
+      <c r="D16" s="40" t="s">
         <v>290</v>
       </c>
-      <c r="C16" s="40" t="s">
+      <c r="E16" s="40" t="s">
         <v>291</v>
       </c>
-      <c r="D16" s="40" t="s">
-        <v>292</v>
-      </c>
-      <c r="E16" s="40" t="s">
-        <v>293</v>
-      </c>
       <c r="G16" s="18" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="I16" s="18" t="b">
         <v>0</v>
@@ -5603,33 +5603,33 @@
     <row r="17" spans="1:10">
       <c r="B17" s="72"/>
       <c r="C17" s="40" t="s">
+        <v>292</v>
+      </c>
+      <c r="D17" s="40" t="s">
+        <v>293</v>
+      </c>
+      <c r="E17" s="40" t="s">
         <v>294</v>
-      </c>
-      <c r="D17" s="40" t="s">
-        <v>295</v>
-      </c>
-      <c r="E17" s="40" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="B18" s="71" t="s">
+        <v>295</v>
+      </c>
+      <c r="C18" s="40" t="s">
+        <v>296</v>
+      </c>
+      <c r="D18" s="40" t="s">
         <v>297</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="E18" s="40" t="s">
         <v>298</v>
       </c>
-      <c r="D18" s="40" t="s">
-        <v>299</v>
-      </c>
-      <c r="E18" s="40" t="s">
-        <v>300</v>
-      </c>
       <c r="G18" s="18" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="I18" s="18" t="b">
         <v>0</v>
@@ -5641,19 +5641,19 @@
     <row r="19" spans="1:10">
       <c r="B19" s="72"/>
       <c r="C19" s="40" t="s">
+        <v>299</v>
+      </c>
+      <c r="D19" s="40" t="s">
+        <v>300</v>
+      </c>
+      <c r="E19" s="40" t="s">
         <v>301</v>
       </c>
-      <c r="D19" s="40" t="s">
-        <v>302</v>
-      </c>
-      <c r="E19" s="40" t="s">
-        <v>303</v>
-      </c>
       <c r="G19" s="18" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="H19" s="18" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="I19" s="18" t="b">
         <v>0</v>
@@ -5664,94 +5664,94 @@
     </row>
     <row r="20" spans="1:10">
       <c r="B20" s="71" t="s">
+        <v>302</v>
+      </c>
+      <c r="C20" s="40" t="s">
+        <v>303</v>
+      </c>
+      <c r="D20" s="40" t="s">
         <v>304</v>
       </c>
-      <c r="C20" s="40" t="s">
+      <c r="E20" s="40" t="s">
         <v>305</v>
-      </c>
-      <c r="D20" s="40" t="s">
-        <v>306</v>
-      </c>
-      <c r="E20" s="40" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="B21" s="72"/>
       <c r="C21" s="40" t="s">
+        <v>306</v>
+      </c>
+      <c r="D21" s="40" t="s">
+        <v>307</v>
+      </c>
+      <c r="E21" s="40" t="s">
         <v>308</v>
-      </c>
-      <c r="D21" s="40" t="s">
-        <v>309</v>
-      </c>
-      <c r="E21" s="40" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="B22" s="41" t="s">
+        <v>309</v>
+      </c>
+      <c r="C22" s="40" t="s">
+        <v>310</v>
+      </c>
+      <c r="D22" s="40" t="s">
         <v>311</v>
       </c>
-      <c r="C22" s="40" t="s">
+      <c r="E22" s="40" t="s">
         <v>312</v>
-      </c>
-      <c r="D22" s="40" t="s">
-        <v>313</v>
-      </c>
-      <c r="E22" s="40" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="B23" s="41" t="s">
+        <v>313</v>
+      </c>
+      <c r="C23" s="40" t="s">
+        <v>314</v>
+      </c>
+      <c r="D23" s="40" t="s">
         <v>315</v>
       </c>
-      <c r="C23" s="40" t="s">
+      <c r="E23" s="40" t="s">
         <v>316</v>
-      </c>
-      <c r="D23" s="40" t="s">
-        <v>317</v>
-      </c>
-      <c r="E23" s="40" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="B24" s="71" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C24" s="40" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D24" s="40" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E24" s="40" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="B25" s="73"/>
       <c r="C25" s="40" t="s">
+        <v>319</v>
+      </c>
+      <c r="D25" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="E25" s="40" t="s">
         <v>321</v>
-      </c>
-      <c r="D25" s="40" t="s">
-        <v>322</v>
-      </c>
-      <c r="E25" s="40" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="B26" s="72"/>
       <c r="C26" s="40" t="s">
+        <v>322</v>
+      </c>
+      <c r="D26" s="40" t="s">
+        <v>323</v>
+      </c>
+      <c r="E26" s="40" t="s">
         <v>324</v>
-      </c>
-      <c r="D26" s="40" t="s">
-        <v>325</v>
-      </c>
-      <c r="E26" s="40" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -5759,7 +5759,7 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="25" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -5770,350 +5770,350 @@
     </row>
     <row r="34" spans="2:5">
       <c r="B34" s="44" t="s">
+        <v>326</v>
+      </c>
+      <c r="C34" s="44" t="s">
+        <v>327</v>
+      </c>
+      <c r="D34" s="44" t="s">
         <v>328</v>
       </c>
-      <c r="C34" s="44" t="s">
+      <c r="E34" s="44" t="s">
         <v>329</v>
-      </c>
-      <c r="D34" s="44" t="s">
-        <v>330</v>
-      </c>
-      <c r="E34" s="44" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="68" t="s">
+        <v>330</v>
+      </c>
+      <c r="C35" s="40" t="s">
+        <v>331</v>
+      </c>
+      <c r="D35" s="40" t="s">
         <v>332</v>
       </c>
-      <c r="C35" s="40" t="s">
+      <c r="E35" s="40" t="s">
         <v>333</v>
-      </c>
-      <c r="D35" s="40" t="s">
-        <v>334</v>
-      </c>
-      <c r="E35" s="40" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="36" spans="2:5">
       <c r="B36" s="69"/>
       <c r="C36" s="40" t="s">
+        <v>334</v>
+      </c>
+      <c r="D36" s="40" t="s">
+        <v>335</v>
+      </c>
+      <c r="E36" s="40" t="s">
         <v>336</v>
-      </c>
-      <c r="D36" s="40" t="s">
-        <v>337</v>
-      </c>
-      <c r="E36" s="40" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="37" spans="2:5">
       <c r="B37" s="69"/>
       <c r="C37" s="40" t="s">
+        <v>337</v>
+      </c>
+      <c r="D37" s="40" t="s">
+        <v>338</v>
+      </c>
+      <c r="E37" s="40" t="s">
         <v>339</v>
-      </c>
-      <c r="D37" s="40" t="s">
-        <v>340</v>
-      </c>
-      <c r="E37" s="40" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="38" spans="2:5">
       <c r="B38" s="69"/>
       <c r="C38" s="40" t="s">
+        <v>340</v>
+      </c>
+      <c r="D38" s="40" t="s">
+        <v>341</v>
+      </c>
+      <c r="E38" s="40" t="s">
         <v>342</v>
-      </c>
-      <c r="D38" s="40" t="s">
-        <v>343</v>
-      </c>
-      <c r="E38" s="40" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="39" spans="2:5">
       <c r="B39" s="69"/>
       <c r="C39" s="40" t="s">
+        <v>343</v>
+      </c>
+      <c r="D39" s="40" t="s">
+        <v>344</v>
+      </c>
+      <c r="E39" s="40" t="s">
         <v>345</v>
-      </c>
-      <c r="D39" s="40" t="s">
-        <v>346</v>
-      </c>
-      <c r="E39" s="40" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="40" spans="2:5">
       <c r="B40" s="70"/>
       <c r="C40" s="40" t="s">
+        <v>346</v>
+      </c>
+      <c r="D40" s="40" t="s">
+        <v>347</v>
+      </c>
+      <c r="E40" s="40" t="s">
         <v>348</v>
-      </c>
-      <c r="D40" s="40" t="s">
-        <v>349</v>
-      </c>
-      <c r="E40" s="40" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="41" spans="2:5">
       <c r="B41" s="68" t="s">
+        <v>349</v>
+      </c>
+      <c r="C41" s="40" t="s">
+        <v>350</v>
+      </c>
+      <c r="D41" s="40" t="s">
         <v>351</v>
       </c>
-      <c r="C41" s="40" t="s">
+      <c r="E41" s="40" t="s">
         <v>352</v>
-      </c>
-      <c r="D41" s="40" t="s">
-        <v>353</v>
-      </c>
-      <c r="E41" s="40" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="42" spans="2:5">
       <c r="B42" s="69"/>
       <c r="C42" s="40" t="s">
+        <v>353</v>
+      </c>
+      <c r="D42" s="40" t="s">
+        <v>354</v>
+      </c>
+      <c r="E42" s="40" t="s">
         <v>355</v>
-      </c>
-      <c r="D42" s="40" t="s">
-        <v>356</v>
-      </c>
-      <c r="E42" s="40" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="43" spans="2:5">
       <c r="B43" s="69"/>
       <c r="C43" s="40" t="s">
+        <v>356</v>
+      </c>
+      <c r="D43" s="40" t="s">
+        <v>357</v>
+      </c>
+      <c r="E43" s="40" t="s">
         <v>358</v>
-      </c>
-      <c r="D43" s="40" t="s">
-        <v>359</v>
-      </c>
-      <c r="E43" s="40" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="44" spans="2:5">
       <c r="B44" s="69"/>
       <c r="C44" s="40" t="s">
+        <v>359</v>
+      </c>
+      <c r="D44" s="40" t="s">
+        <v>360</v>
+      </c>
+      <c r="E44" s="40" t="s">
         <v>361</v>
-      </c>
-      <c r="D44" s="40" t="s">
-        <v>362</v>
-      </c>
-      <c r="E44" s="40" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="45" spans="2:5">
       <c r="B45" s="69"/>
       <c r="C45" s="40" t="s">
+        <v>362</v>
+      </c>
+      <c r="D45" s="40" t="s">
+        <v>363</v>
+      </c>
+      <c r="E45" s="40" t="s">
         <v>364</v>
-      </c>
-      <c r="D45" s="40" t="s">
-        <v>365</v>
-      </c>
-      <c r="E45" s="40" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="46" spans="2:5">
       <c r="B46" s="70"/>
       <c r="C46" s="40" t="s">
+        <v>365</v>
+      </c>
+      <c r="D46" s="40" t="s">
+        <v>366</v>
+      </c>
+      <c r="E46" s="40" t="s">
         <v>367</v>
-      </c>
-      <c r="D46" s="40" t="s">
-        <v>368</v>
-      </c>
-      <c r="E46" s="40" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="47" spans="2:5">
       <c r="B47" s="68" t="s">
+        <v>368</v>
+      </c>
+      <c r="C47" s="40" t="s">
+        <v>369</v>
+      </c>
+      <c r="D47" s="40" t="s">
         <v>370</v>
       </c>
-      <c r="C47" s="40" t="s">
+      <c r="E47" s="40" t="s">
         <v>371</v>
-      </c>
-      <c r="D47" s="40" t="s">
-        <v>372</v>
-      </c>
-      <c r="E47" s="40" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="48" spans="2:5">
       <c r="B48" s="69"/>
       <c r="C48" s="40" t="s">
+        <v>372</v>
+      </c>
+      <c r="D48" s="40" t="s">
+        <v>373</v>
+      </c>
+      <c r="E48" s="40" t="s">
         <v>374</v>
-      </c>
-      <c r="D48" s="40" t="s">
-        <v>375</v>
-      </c>
-      <c r="E48" s="40" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="49" spans="2:5">
       <c r="B49" s="69"/>
       <c r="C49" s="40" t="s">
+        <v>375</v>
+      </c>
+      <c r="D49" s="40" t="s">
+        <v>376</v>
+      </c>
+      <c r="E49" s="40" t="s">
         <v>377</v>
-      </c>
-      <c r="D49" s="40" t="s">
-        <v>378</v>
-      </c>
-      <c r="E49" s="40" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="50" spans="2:5">
       <c r="B50" s="69"/>
       <c r="C50" s="40" t="s">
+        <v>378</v>
+      </c>
+      <c r="D50" s="40" t="s">
+        <v>379</v>
+      </c>
+      <c r="E50" s="40" t="s">
         <v>380</v>
-      </c>
-      <c r="D50" s="40" t="s">
-        <v>381</v>
-      </c>
-      <c r="E50" s="40" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="51" spans="2:5">
       <c r="B51" s="69"/>
       <c r="C51" s="40" t="s">
+        <v>381</v>
+      </c>
+      <c r="D51" s="40" t="s">
+        <v>382</v>
+      </c>
+      <c r="E51" s="40" t="s">
         <v>383</v>
-      </c>
-      <c r="D51" s="40" t="s">
-        <v>384</v>
-      </c>
-      <c r="E51" s="40" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="52" spans="2:5">
       <c r="B52" s="70"/>
       <c r="C52" s="40" t="s">
+        <v>384</v>
+      </c>
+      <c r="D52" s="40" t="s">
+        <v>385</v>
+      </c>
+      <c r="E52" s="40" t="s">
         <v>386</v>
-      </c>
-      <c r="D52" s="40" t="s">
-        <v>387</v>
-      </c>
-      <c r="E52" s="40" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="53" spans="2:5">
       <c r="B53" s="68" t="s">
+        <v>387</v>
+      </c>
+      <c r="C53" s="40" t="s">
+        <v>388</v>
+      </c>
+      <c r="D53" s="40" t="s">
         <v>389</v>
       </c>
-      <c r="C53" s="40" t="s">
+      <c r="E53" s="40" t="s">
         <v>390</v>
-      </c>
-      <c r="D53" s="40" t="s">
-        <v>391</v>
-      </c>
-      <c r="E53" s="40" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="54" spans="2:5">
       <c r="B54" s="69"/>
       <c r="C54" s="40" t="s">
+        <v>391</v>
+      </c>
+      <c r="D54" s="40" t="s">
+        <v>392</v>
+      </c>
+      <c r="E54" s="40" t="s">
         <v>393</v>
-      </c>
-      <c r="D54" s="40" t="s">
-        <v>394</v>
-      </c>
-      <c r="E54" s="40" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="55" spans="2:5">
       <c r="B55" s="69"/>
       <c r="C55" s="40" t="s">
+        <v>394</v>
+      </c>
+      <c r="D55" s="40" t="s">
+        <v>395</v>
+      </c>
+      <c r="E55" s="40" t="s">
         <v>396</v>
-      </c>
-      <c r="D55" s="40" t="s">
-        <v>397</v>
-      </c>
-      <c r="E55" s="40" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="56" spans="2:5">
       <c r="B56" s="69"/>
       <c r="C56" s="40" t="s">
+        <v>397</v>
+      </c>
+      <c r="D56" s="40" t="s">
+        <v>398</v>
+      </c>
+      <c r="E56" s="40" t="s">
         <v>399</v>
-      </c>
-      <c r="D56" s="40" t="s">
-        <v>400</v>
-      </c>
-      <c r="E56" s="40" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="57" spans="2:5">
       <c r="B57" s="70"/>
       <c r="C57" s="40" t="s">
+        <v>400</v>
+      </c>
+      <c r="D57" s="40" t="s">
+        <v>401</v>
+      </c>
+      <c r="E57" s="40" t="s">
         <v>402</v>
-      </c>
-      <c r="D57" s="40" t="s">
-        <v>403</v>
-      </c>
-      <c r="E57" s="40" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="58" spans="2:5">
       <c r="B58" s="68" t="s">
+        <v>403</v>
+      </c>
+      <c r="C58" s="40" t="s">
+        <v>404</v>
+      </c>
+      <c r="D58" s="40" t="s">
         <v>405</v>
       </c>
-      <c r="C58" s="40" t="s">
+      <c r="E58" s="40" t="s">
         <v>406</v>
-      </c>
-      <c r="D58" s="40" t="s">
-        <v>407</v>
-      </c>
-      <c r="E58" s="40" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="59" spans="2:5">
       <c r="B59" s="69"/>
       <c r="C59" s="40" t="s">
+        <v>407</v>
+      </c>
+      <c r="D59" s="40" t="s">
+        <v>408</v>
+      </c>
+      <c r="E59" s="40" t="s">
         <v>409</v>
-      </c>
-      <c r="D59" s="40" t="s">
-        <v>410</v>
-      </c>
-      <c r="E59" s="40" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="60" spans="2:5">
       <c r="B60" s="69"/>
       <c r="C60" s="40" t="s">
+        <v>410</v>
+      </c>
+      <c r="D60" s="40" t="s">
+        <v>411</v>
+      </c>
+      <c r="E60" s="40" t="s">
         <v>412</v>
-      </c>
-      <c r="D60" s="40" t="s">
-        <v>413</v>
-      </c>
-      <c r="E60" s="40" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="61" spans="2:5">
       <c r="B61" s="70"/>
       <c r="C61" s="40" t="s">
+        <v>413</v>
+      </c>
+      <c r="D61" s="40" t="s">
+        <v>414</v>
+      </c>
+      <c r="E61" s="40" t="s">
         <v>415</v>
-      </c>
-      <c r="D61" s="40" t="s">
-        <v>416</v>
-      </c>
-      <c r="E61" s="40" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="62" spans="2:5">
@@ -6421,7 +6421,7 @@
   </sheetPr>
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="23"/>
   <cols>
@@ -6455,7 +6455,7 @@
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:1">
@@ -6505,7 +6505,7 @@
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="36" spans="1:1">
@@ -6525,145 +6525,145 @@
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="17" t="s">
-        <v>143</v>
+        <v>447</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E51" s="22" t="s">
-        <v>173</v>
+        <v>448</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" s="17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" s="17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" s="18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" s="18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96" s="18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" s="18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -7025,7 +7025,7 @@
         <v>204</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C5" s="34">
         <v>1</v>

</xml_diff>